<commit_message>
final TAAK1-grades, feedback, files
</commit_message>
<xml_diff>
--- a/MVandebroek/TAKEN/ATSTAT-TASKS/TASK1/1.FILES/overallgrades_all_taak1.xlsx
+++ b/MVandebroek/TAKEN/ATSTAT-TASKS/TASK1/1.FILES/overallgrades_all_taak1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/leonard_maaya_kuleuven_be1/Documents/ATSTAT-TASKS/TASK1/1.FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_138A9DCD8F79A8D366075C52F37BD272FAC42213" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{776F7CA3-4155-4B0A-87F8-5AF63163B59C}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="11_329A9DCD8F79A8D366075C52F37BD2725AC264DF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3A0941F-FD8E-4B45-A257-4B5A9ECE4746}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,27 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$358</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$358</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2518" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="1347">
   <si>
     <t>User.Name</t>
   </si>
@@ -4058,6 +4071,12 @@
   </si>
   <si>
     <t>2023-10-19 16:12:58</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -4081,12 +4100,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4101,11 +4126,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4444,15 +4472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y358"/>
+  <dimension ref="A1:Z358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M215" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K360" sqref="K360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4529,7 +4557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4593,8 +4621,11 @@
       <c r="Y2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4671,7 +4702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4748,7 +4779,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -4813,7 +4844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -4884,7 +4915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -4949,7 +4980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -5014,7 +5045,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -5091,7 +5122,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -5168,7 +5199,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -5245,7 +5276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -5310,7 +5341,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -5353,8 +5384,8 @@
       <c r="N13">
         <v>23.02</v>
       </c>
-      <c r="O13">
-        <v>0</v>
+      <c r="O13" s="3">
+        <v>0.75</v>
       </c>
       <c r="P13">
         <v>15</v>
@@ -5377,14 +5408,14 @@
       <c r="W13">
         <v>1</v>
       </c>
-      <c r="X13">
-        <v>2</v>
+      <c r="X13" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -5461,7 +5492,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -5538,7 +5569,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -5569,8 +5600,8 @@
       <c r="J16">
         <v>86631.657000000007</v>
       </c>
-      <c r="K16">
-        <v>0</v>
+      <c r="K16" s="3">
+        <v>1</v>
       </c>
       <c r="L16">
         <v>11</v>
@@ -5590,8 +5621,8 @@
       <c r="Q16">
         <v>1</v>
       </c>
-      <c r="R16">
-        <v>1</v>
+      <c r="R16" t="s">
+        <v>1345</v>
       </c>
       <c r="S16">
         <v>1</v>
@@ -5608,8 +5639,8 @@
       <c r="W16">
         <v>1</v>
       </c>
-      <c r="X16">
-        <v>3</v>
+      <c r="X16" s="3">
+        <v>4</v>
       </c>
       <c r="Y16" t="s">
         <v>41</v>
@@ -6300,8 +6331,8 @@
       <c r="N26">
         <v>5.9059999999999997</v>
       </c>
-      <c r="O26">
-        <v>0</v>
+      <c r="O26" s="3">
+        <v>0.75</v>
       </c>
       <c r="P26">
         <v>13</v>
@@ -6327,8 +6358,8 @@
       <c r="W26">
         <v>0</v>
       </c>
-      <c r="X26">
-        <v>2</v>
+      <c r="X26" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y26" t="s">
         <v>41</v>
@@ -7647,8 +7678,8 @@
       <c r="J44">
         <v>47489.495000000003</v>
       </c>
-      <c r="K44">
-        <v>0</v>
+      <c r="K44" s="3">
+        <v>1</v>
       </c>
       <c r="L44">
         <v>9</v>
@@ -7659,8 +7690,8 @@
       <c r="N44">
         <v>8.4480000000000004</v>
       </c>
-      <c r="O44">
-        <v>0</v>
+      <c r="O44" s="3">
+        <v>1</v>
       </c>
       <c r="P44">
         <v>13</v>
@@ -7686,8 +7717,8 @@
       <c r="W44">
         <v>1</v>
       </c>
-      <c r="X44">
-        <v>1</v>
+      <c r="X44" s="3">
+        <v>3</v>
       </c>
       <c r="Y44" t="s">
         <v>41</v>
@@ -7736,8 +7767,8 @@
       <c r="N45">
         <v>0.42699999999999999</v>
       </c>
-      <c r="O45">
-        <v>0</v>
+      <c r="O45" s="3">
+        <v>0.75</v>
       </c>
       <c r="P45">
         <v>13</v>
@@ -7763,8 +7794,8 @@
       <c r="W45">
         <v>1</v>
       </c>
-      <c r="X45">
-        <v>3</v>
+      <c r="X45" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y45" t="s">
         <v>41</v>
@@ -8020,8 +8051,8 @@
       <c r="N49">
         <v>12.884</v>
       </c>
-      <c r="O49">
-        <v>0</v>
+      <c r="O49" s="3">
+        <v>0.75</v>
       </c>
       <c r="P49">
         <v>15</v>
@@ -8047,8 +8078,8 @@
       <c r="W49">
         <v>0</v>
       </c>
-      <c r="X49">
-        <v>2</v>
+      <c r="X49" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y49" t="s">
         <v>41</v>
@@ -8280,26 +8311,26 @@
       <c r="H53">
         <v>4</v>
       </c>
-      <c r="I53">
-        <v>2.7E-2</v>
+      <c r="I53" s="3">
+        <v>86335.37</v>
       </c>
       <c r="J53">
         <v>86335.370999999999</v>
       </c>
-      <c r="K53">
-        <v>0</v>
+      <c r="K53" s="3">
+        <v>1</v>
       </c>
       <c r="L53">
         <v>10</v>
       </c>
-      <c r="M53">
-        <v>86335.37</v>
+      <c r="M53" s="3">
+        <v>2.7E-2</v>
       </c>
       <c r="N53">
         <v>2.7E-2</v>
       </c>
-      <c r="O53">
-        <v>0</v>
+      <c r="O53" s="3">
+        <v>1</v>
       </c>
       <c r="P53">
         <v>15</v>
@@ -8325,8 +8356,8 @@
       <c r="W53">
         <v>1</v>
       </c>
-      <c r="X53">
-        <v>2</v>
+      <c r="X53" s="3">
+        <v>4</v>
       </c>
       <c r="Y53" t="s">
         <v>41</v>
@@ -10033,8 +10064,8 @@
       <c r="N76">
         <v>2.7959999999999998</v>
       </c>
-      <c r="O76">
-        <v>0</v>
+      <c r="O76" s="3">
+        <v>0.75</v>
       </c>
       <c r="P76">
         <v>13</v>
@@ -10060,8 +10091,8 @@
       <c r="W76">
         <v>1</v>
       </c>
-      <c r="X76">
-        <v>3</v>
+      <c r="X76" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y76" t="s">
         <v>41</v>
@@ -10098,20 +10129,20 @@
       <c r="J77">
         <v>49126.55</v>
       </c>
-      <c r="K77">
-        <v>0</v>
+      <c r="K77" s="3">
+        <v>0.5</v>
       </c>
       <c r="L77">
         <v>8</v>
       </c>
-      <c r="M77">
+      <c r="M77" s="4">
         <v>3933</v>
       </c>
       <c r="N77">
         <v>3.9329999999999998</v>
       </c>
-      <c r="O77">
-        <v>0</v>
+      <c r="O77" s="3">
+        <v>1</v>
       </c>
       <c r="P77">
         <v>16</v>
@@ -10137,8 +10168,8 @@
       <c r="W77">
         <v>1</v>
       </c>
-      <c r="X77">
-        <v>1</v>
+      <c r="X77" s="3">
+        <v>2.5</v>
       </c>
       <c r="Y77" t="s">
         <v>41</v>
@@ -10483,8 +10514,8 @@
       <c r="N82">
         <v>9.68</v>
       </c>
-      <c r="O82">
-        <v>0</v>
+      <c r="O82" s="3">
+        <v>0.25</v>
       </c>
       <c r="P82">
         <v>16</v>
@@ -10510,8 +10541,8 @@
       <c r="W82">
         <v>1</v>
       </c>
-      <c r="X82">
-        <v>3</v>
+      <c r="X82" s="3">
+        <v>3.25</v>
       </c>
       <c r="Y82" t="s">
         <v>41</v>
@@ -11928,8 +11959,8 @@
       <c r="N101">
         <v>30.457999999999998</v>
       </c>
-      <c r="O101">
-        <v>0</v>
+      <c r="O101" s="3">
+        <v>1</v>
       </c>
       <c r="P101">
         <v>15</v>
@@ -11955,8 +11986,8 @@
       <c r="W101">
         <v>0</v>
       </c>
-      <c r="X101">
-        <v>2</v>
+      <c r="X101" s="3">
+        <v>3</v>
       </c>
       <c r="Y101" t="s">
         <v>41</v>
@@ -12742,8 +12773,8 @@
       <c r="N112">
         <v>3.4489999999999998</v>
       </c>
-      <c r="O112">
-        <v>0</v>
+      <c r="O112" s="3">
+        <v>0.75</v>
       </c>
       <c r="P112">
         <v>14</v>
@@ -12769,8 +12800,8 @@
       <c r="W112">
         <v>0</v>
       </c>
-      <c r="X112">
-        <v>2</v>
+      <c r="X112" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y112" t="s">
         <v>41</v>
@@ -13180,8 +13211,8 @@
       <c r="N118">
         <v>20.550999999999998</v>
       </c>
-      <c r="O118">
-        <v>0</v>
+      <c r="O118" s="3">
+        <v>0.25</v>
       </c>
       <c r="P118">
         <v>14</v>
@@ -13207,8 +13238,8 @@
       <c r="W118">
         <v>0</v>
       </c>
-      <c r="X118">
-        <v>1</v>
+      <c r="X118" s="3">
+        <v>1.25</v>
       </c>
       <c r="Y118" t="s">
         <v>41</v>
@@ -13257,8 +13288,8 @@
       <c r="N119">
         <v>10.901</v>
       </c>
-      <c r="O119">
-        <v>0</v>
+      <c r="O119" s="3">
+        <v>0.75</v>
       </c>
       <c r="P119">
         <v>14</v>
@@ -13284,8 +13315,8 @@
       <c r="W119">
         <v>1</v>
       </c>
-      <c r="X119">
-        <v>3</v>
+      <c r="X119" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y119" t="s">
         <v>41</v>
@@ -13895,10 +13926,10 @@
         <v>0</v>
       </c>
       <c r="W127">
-        <v>0</v>
-      </c>
-      <c r="X127">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="X127" s="3">
+        <v>4</v>
       </c>
       <c r="Y127" t="s">
         <v>41</v>
@@ -14859,8 +14890,8 @@
       <c r="N140">
         <v>194.05500000000001</v>
       </c>
-      <c r="O140">
-        <v>0</v>
+      <c r="O140" s="3">
+        <v>0.75</v>
       </c>
       <c r="P140">
         <v>16</v>
@@ -14886,8 +14917,8 @@
       <c r="W140">
         <v>0</v>
       </c>
-      <c r="X140">
-        <v>2</v>
+      <c r="X140" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y140" t="s">
         <v>41</v>
@@ -15081,8 +15112,8 @@
       <c r="N143">
         <v>1.2490000000000001</v>
       </c>
-      <c r="O143">
-        <v>0</v>
+      <c r="O143" s="3">
+        <v>0.75</v>
       </c>
       <c r="P143">
         <v>13</v>
@@ -15108,8 +15139,8 @@
       <c r="W143">
         <v>0</v>
       </c>
-      <c r="X143">
-        <v>2</v>
+      <c r="X143" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y143" t="s">
         <v>41</v>
@@ -17204,8 +17235,8 @@
       <c r="N171">
         <v>86.067999999999998</v>
       </c>
-      <c r="O171">
-        <v>0</v>
+      <c r="O171" s="3">
+        <v>0.75</v>
       </c>
       <c r="P171">
         <v>13</v>
@@ -17231,8 +17262,8 @@
       <c r="W171">
         <v>1</v>
       </c>
-      <c r="X171">
-        <v>3</v>
+      <c r="X171" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y171" t="s">
         <v>41</v>
@@ -20052,8 +20083,8 @@
       <c r="J209">
         <v>45621.792000000001</v>
       </c>
-      <c r="K209">
-        <v>0</v>
+      <c r="K209" s="3">
+        <v>0.5</v>
       </c>
       <c r="L209">
         <v>8</v>
@@ -20091,8 +20122,8 @@
       <c r="W209">
         <v>1</v>
       </c>
-      <c r="X209">
-        <v>2</v>
+      <c r="X209" s="3">
+        <v>2.5</v>
       </c>
       <c r="Y209" t="s">
         <v>41</v>
@@ -23908,11 +23939,11 @@
       <c r="V259">
         <v>0</v>
       </c>
-      <c r="W259">
-        <v>0</v>
-      </c>
-      <c r="X259">
-        <v>2</v>
+      <c r="W259" s="3">
+        <v>1</v>
+      </c>
+      <c r="X259" s="3">
+        <v>3</v>
       </c>
       <c r="Y259" t="s">
         <v>41</v>
@@ -25379,8 +25410,8 @@
       <c r="N279">
         <v>1.7370000000000001</v>
       </c>
-      <c r="O279">
-        <v>0</v>
+      <c r="O279" s="3">
+        <v>0.75</v>
       </c>
       <c r="P279">
         <v>13</v>
@@ -25406,8 +25437,8 @@
       <c r="W279">
         <v>1</v>
       </c>
-      <c r="X279">
-        <v>2</v>
+      <c r="X279" s="3">
+        <v>2.75</v>
       </c>
       <c r="Y279" t="s">
         <v>41</v>
@@ -25456,8 +25487,8 @@
       <c r="N280">
         <v>64.605000000000004</v>
       </c>
-      <c r="O280">
-        <v>0</v>
+      <c r="O280" s="3">
+        <v>0.75</v>
       </c>
       <c r="P280">
         <v>15</v>
@@ -25483,8 +25514,8 @@
       <c r="W280">
         <v>0</v>
       </c>
-      <c r="X280">
-        <v>1</v>
+      <c r="X280" s="3">
+        <v>1.75</v>
       </c>
       <c r="Y280" t="s">
         <v>41</v>
@@ -25610,8 +25641,8 @@
       <c r="N282">
         <v>144.54900000000001</v>
       </c>
-      <c r="O282">
-        <v>0</v>
+      <c r="O282" s="3">
+        <v>0.75</v>
       </c>
       <c r="P282">
         <v>13</v>
@@ -25637,8 +25668,8 @@
       <c r="W282">
         <v>1</v>
       </c>
-      <c r="X282">
-        <v>3</v>
+      <c r="X282" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y282" t="s">
         <v>41</v>
@@ -25841,8 +25872,8 @@
       <c r="N285">
         <v>91.828000000000003</v>
       </c>
-      <c r="O285">
-        <v>0</v>
+      <c r="O285" s="3">
+        <v>0.75</v>
       </c>
       <c r="P285">
         <v>13</v>
@@ -25868,8 +25899,8 @@
       <c r="W285">
         <v>1</v>
       </c>
-      <c r="X285">
-        <v>3</v>
+      <c r="X285" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y285" t="s">
         <v>41</v>
@@ -27203,8 +27234,8 @@
       <c r="N303">
         <v>25.608000000000001</v>
       </c>
-      <c r="O303">
-        <v>0</v>
+      <c r="O303" s="3">
+        <v>0.75</v>
       </c>
       <c r="P303">
         <v>16</v>
@@ -27230,8 +27261,8 @@
       <c r="W303">
         <v>1</v>
       </c>
-      <c r="X303">
-        <v>3</v>
+      <c r="X303" s="3">
+        <v>3.75</v>
       </c>
       <c r="Y303" t="s">
         <v>41</v>
@@ -28843,8 +28874,8 @@
       <c r="N325">
         <v>102.509</v>
       </c>
-      <c r="O325">
-        <v>0</v>
+      <c r="O325" s="3">
+        <v>0.25</v>
       </c>
       <c r="P325">
         <v>15</v>
@@ -28870,8 +28901,8 @@
       <c r="W325">
         <v>0</v>
       </c>
-      <c r="X325">
-        <v>2</v>
+      <c r="X325" s="3">
+        <v>2.25</v>
       </c>
       <c r="Y325" t="s">
         <v>41</v>
@@ -30619,11 +30650,11 @@
       <c r="V349">
         <v>0</v>
       </c>
-      <c r="W349">
-        <v>0</v>
-      </c>
-      <c r="X349">
-        <v>2</v>
+      <c r="W349" s="2">
+        <v>1</v>
+      </c>
+      <c r="X349" s="2">
+        <v>3</v>
       </c>
       <c r="Y349" t="s">
         <v>41</v>
@@ -31255,8 +31286,8 @@
       <c r="N358">
         <v>0.04</v>
       </c>
-      <c r="O358">
-        <v>0</v>
+      <c r="O358" s="3">
+        <v>0.25</v>
       </c>
       <c r="P358">
         <v>15</v>
@@ -31282,15 +31313,16 @@
       <c r="W358">
         <v>1</v>
       </c>
-      <c r="X358">
-        <v>3</v>
+      <c r="X358" s="3">
+        <v>3.25</v>
       </c>
       <c r="Y358" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y358" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Z358" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>